<commit_message>
added datasource files from census
</commit_message>
<xml_diff>
--- a/project_information/Project Tracking Sheet.xlsx
+++ b/project_information/Project Tracking Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hcgroupnet-my.sharepoint.com/personal/matthew_vella_hanson_com_au/Documents/Documents/Data Analytics/UWA Bootcamp/Coursework/Project 1/exploration-of-food-in-perth/project_information/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_F25DC773A252ABDACC1048D3999C6D3E5BDE58F8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6437AA6E-9FC6-4AD0-BC2A-650AED589072}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="11_F25DC773A252ABDACC1048D3999C6D3E5BDE58F8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7CF7CD62-17C1-4941-BB42-124A8B08C9AB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="285" windowWidth="29040" windowHeight="17415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="285" windowWidth="29040" windowHeight="17415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -47,6 +47,14 @@
       <u/>
       <sz val="20"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -69,14 +77,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -355,18 +366,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>